<commit_message>
MS XL Addin updates in function names + documentation
</commit_message>
<xml_diff>
--- a/templates/SurplusLinesTax-Test-Template.xlsx
+++ b/templates/SurplusLinesTax-Test-Template.xlsx
@@ -589,7 +589,7 @@
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
         <is>
-          <t>Detailed Breakdown (SLTAX.DETAILS)</t>
+          <t>Detailed Breakdown (SLTAX.CALCULATE_DETAILS)</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
         <v>10000</v>
       </c>
       <c r="C13">
-        <f>SLTAX.DETAILS(A13, B13)</f>
+        <f>SLTAX.CALCULATE_DETAILS(A13, B13)</f>
         <v/>
       </c>
     </row>
@@ -649,14 +649,14 @@
         <v>25000</v>
       </c>
       <c r="C14">
-        <f>SLTAX.DETAILS(A14, B14)</f>
+        <f>SLTAX.CALCULATE_DETAILS(A14, B14)</f>
         <v/>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Compact View (SLTAX.WITHPREMIUM)</t>
+          <t>Compact View (SLTAX.CALCULATE_WITHPREMIUM)</t>
         </is>
       </c>
     </row>
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="B19">
-        <f>SLTAX.WITHPREMIUM("Florida", 15000)</f>
+        <f>SLTAX.CALCULATE_WITHPREMIUM("Florida", 15000)</f>
         <v/>
       </c>
     </row>
@@ -915,7 +915,7 @@
     <row r="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>Complete Rate Details (SLTAX.RATESDETAILS)</t>
+          <t>Complete Rate Details (SLTAX.RATES_DETAILS)</t>
         </is>
       </c>
     </row>
@@ -978,7 +978,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <f>SLTAX.RATESDETAILS()</f>
+        <f>SLTAX.RATES_DETAILS()</f>
         <v/>
       </c>
     </row>
@@ -1167,7 +1167,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <f>SLTAX.HISTORICALRATEDETAILS("Texas", "2024-01-01")</f>
+        <f>SLTAX.HISTORICALRATE_DETAILS("Texas", "2024-01-01")</f>
         <v/>
       </c>
     </row>
@@ -1180,7 +1180,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <f>SLTAX.HISTORICALRATEDETAILS("Texas", "2024-01-01", TRUE)</f>
+        <f>SLTAX.HISTORICALRATE_DETAILS("Texas", "2024-01-01", TRUE)</f>
         <v/>
       </c>
     </row>
@@ -1268,7 +1268,7 @@
     <row r="5">
       <c r="A5" s="9" t="inlineStr">
         <is>
-          <t>SLTAX.DETAILS(state, premium, [multiline])</t>
+          <t>SLTAX.CALCULATE_DETAILS(state, premium, [multiline])</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="C5" s="9" t="inlineStr">
         <is>
-          <t>SLTAX.DETAILS("CA", 10000)</t>
+          <t>SLTAX.CALCULATE_DETAILS("CA", 10000)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1290,7 +1290,7 @@
     <row r="6">
       <c r="A6" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.WITHPREMIUM(state, premium)</t>
+          <t>SLTAX.CALCULATE_WITHPREMIUM(state, premium)</t>
         </is>
       </c>
       <c r="B6" s="8" t="inlineStr">
@@ -1300,7 +1300,7 @@
       </c>
       <c r="C6" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.WITHPREMIUM("FL", 15000)</t>
+          <t>SLTAX.CALCULATE_WITHPREMIUM("FL", 15000)</t>
         </is>
       </c>
       <c r="D6" s="8" t="inlineStr">
@@ -1378,7 +1378,7 @@
     <row r="10">
       <c r="A10" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.RATESDETAILS()</t>
+          <t>SLTAX.RATES_DETAILS()</t>
         </is>
       </c>
       <c r="B10" s="8" t="inlineStr">
@@ -1388,7 +1388,7 @@
       </c>
       <c r="C10" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.RATESDETAILS()</t>
+          <t>SLTAX.RATES_DETAILS()</t>
         </is>
       </c>
       <c r="D10" s="8" t="inlineStr">
@@ -1422,7 +1422,7 @@
     <row r="12">
       <c r="A12" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.HISTORICALRATEDETAILS(state, date, [multiline])</t>
+          <t>SLTAX.HISTORICALRATE_DETAILS(state, date, [multiline])</t>
         </is>
       </c>
       <c r="B12" s="8" t="inlineStr">
@@ -1432,7 +1432,7 @@
       </c>
       <c r="C12" s="7" t="inlineStr">
         <is>
-          <t>SLTAX.HISTORICALRATEDETAILS("TX", "2024-01-01")</t>
+          <t>SLTAX.HISTORICALRATE_DETAILS("TX", "2024-01-01")</t>
         </is>
       </c>
       <c r="D12" s="8" t="inlineStr">

</xml_diff>